<commit_message>
switched from StAX to XStream lib for deserializing xml added Valutes class to match the XML structure added required XStream annotations to Valutes and Valute classes
</commit_message>
<xml_diff>
--- a/Practice_2.xlsx
+++ b/Practice_2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="299">
   <si>
     <t>ID</t>
   </si>
@@ -34,6 +34,489 @@
     <t>Value</t>
   </si>
   <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>554</t>
+  </si>
+  <si>
+    <t>NZD</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>New Zealand Dollar</t>
+  </si>
+  <si>
+    <t>11.6987</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>934</t>
+  </si>
+  <si>
+    <t>TMT</t>
+  </si>
+  <si>
+    <t>Turkmenistan Manat</t>
+  </si>
+  <si>
+    <t>4.8906</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>Canadian Dollar</t>
+  </si>
+  <si>
+    <t>12.969</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>981</t>
+  </si>
+  <si>
+    <t>GEL</t>
+  </si>
+  <si>
+    <t>Georgian Lar</t>
+  </si>
+  <si>
+    <t>6.4181</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>756</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>Swiss Franc</t>
+  </si>
+  <si>
+    <t>17.4096</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Albanian lek</t>
+  </si>
+  <si>
+    <t>1.5699</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>398</t>
+  </si>
+  <si>
+    <t>KZT</t>
+  </si>
+  <si>
+    <t>Kazakhstan Tenge</t>
+  </si>
+  <si>
+    <t>0.4546</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>840</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>US Dollar</t>
+  </si>
+  <si>
+    <t>17.1171</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>CNY</t>
+  </si>
+  <si>
+    <t>Chinese yuan renminbi</t>
+  </si>
+  <si>
+    <t>2.5385</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>392</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Japanese Yen</t>
+  </si>
+  <si>
+    <t>15.8045</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>348</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>Hungarian Forint</t>
+  </si>
+  <si>
+    <t>6.1386</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>949</t>
+  </si>
+  <si>
+    <t>TRY</t>
+  </si>
+  <si>
+    <t>Turkish Lira</t>
+  </si>
+  <si>
+    <t>3.1455</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>410</t>
+  </si>
+  <si>
+    <t>KRW</t>
+  </si>
+  <si>
+    <t>South Korean won</t>
+  </si>
+  <si>
+    <t>1.5333</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>344</t>
+  </si>
+  <si>
+    <t>HKD</t>
+  </si>
+  <si>
+    <t>Hong Kong dollar</t>
+  </si>
+  <si>
+    <t>2.183</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>980</t>
+  </si>
+  <si>
+    <t>UAH</t>
+  </si>
+  <si>
+    <t>Ukraine Hryvnia</t>
+  </si>
+  <si>
+    <t>0.6092</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>946</t>
+  </si>
+  <si>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>Romanian Leu</t>
+  </si>
+  <si>
+    <t>4.2194</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>356</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>Indian rupee</t>
+  </si>
+  <si>
+    <t>2.4281</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>Czech Koruna</t>
+  </si>
+  <si>
+    <t>0.771</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>985</t>
+  </si>
+  <si>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>Polish Zloty</t>
+  </si>
+  <si>
+    <t>4.5941</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>191</t>
+  </si>
+  <si>
+    <t>HRK</t>
+  </si>
+  <si>
+    <t>Croatian Kuna</t>
+  </si>
+  <si>
+    <t>2.6575</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>352</t>
+  </si>
+  <si>
+    <t>ISK</t>
+  </si>
+  <si>
+    <t>Iceland Krona</t>
+  </si>
+  <si>
+    <t>1.4292</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>784</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>U.A.E. Dirham</t>
+  </si>
+  <si>
+    <t>4.6603</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>578</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>Norwegian Krone</t>
+  </si>
+  <si>
+    <t>2.0248</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>376</t>
+  </si>
+  <si>
+    <t>ILS</t>
+  </si>
+  <si>
+    <t>Shekel Israelit</t>
+  </si>
+  <si>
+    <t>4.6736</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>414</t>
+  </si>
+  <si>
+    <t>KWD</t>
+  </si>
+  <si>
+    <t>Kuwaiti Dinar</t>
+  </si>
+  <si>
+    <t>56.5331</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>972</t>
+  </si>
+  <si>
+    <t>TJS</t>
+  </si>
+  <si>
+    <t>Tajikistan Somoni</t>
+  </si>
+  <si>
+    <t>1.8146</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>933</t>
+  </si>
+  <si>
+    <t>BYN</t>
+  </si>
+  <si>
+    <t>Belarussian Ruble</t>
+  </si>
+  <si>
+    <t>7.9596</t>
+  </si>
+  <si>
+    <t>051</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>Armenian Dram</t>
+  </si>
+  <si>
+    <t>0.3518</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>458</t>
+  </si>
+  <si>
+    <t>MYR</t>
+  </si>
+  <si>
+    <t>Malaysian Ringgit</t>
+  </si>
+  <si>
+    <t>4.18</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>Australian Dollar</t>
+  </si>
+  <si>
+    <t>12.3696</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>807</t>
+  </si>
+  <si>
+    <t>MKD</t>
+  </si>
+  <si>
+    <t>Macedonian denar</t>
+  </si>
+  <si>
+    <t>3.2053</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>941</t>
+  </si>
+  <si>
+    <t>RSD</t>
+  </si>
+  <si>
+    <t>Serbian Dinar</t>
+  </si>
+  <si>
+    <t>16.6691</t>
+  </si>
+  <si>
     <t>47</t>
   </si>
   <si>
@@ -43,28 +526,55 @@
     <t>EUR</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Euro</t>
   </si>
   <si>
     <t>19.7368</t>
   </si>
   <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>840</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>US Dollar</t>
-  </si>
-  <si>
-    <t>17.1171</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>Danish Krone</t>
+  </si>
+  <si>
+    <t>2.6443</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>417</t>
+  </si>
+  <si>
+    <t>KGS</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan Som</t>
+  </si>
+  <si>
+    <t>2.4506</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>752</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>Swedish Krona</t>
+  </si>
+  <si>
+    <t>1.9297</t>
   </si>
   <si>
     <t>36</t>
@@ -82,93 +592,6 @@
     <t>0.2556</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>946</t>
-  </si>
-  <si>
-    <t>RON</t>
-  </si>
-  <si>
-    <t>Romanian Leu</t>
-  </si>
-  <si>
-    <t>4.2194</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>980</t>
-  </si>
-  <si>
-    <t>UAH</t>
-  </si>
-  <si>
-    <t>Ukraine Hryvnia</t>
-  </si>
-  <si>
-    <t>0.6092</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>784</t>
-  </si>
-  <si>
-    <t>AED</t>
-  </si>
-  <si>
-    <t>U.A.E. Dirham</t>
-  </si>
-  <si>
-    <t>4.6603</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Albanian lek</t>
-  </si>
-  <si>
-    <t>1.5699</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>Armenian Dram</t>
-  </si>
-  <si>
-    <t>0.3518</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>AUD</t>
-  </si>
-  <si>
-    <t>Australian Dollar</t>
-  </si>
-  <si>
-    <t>12.3696</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -199,88 +622,34 @@
     <t>10.0911</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>933</t>
-  </si>
-  <si>
-    <t>BYN</t>
-  </si>
-  <si>
-    <t>Belarussian Ruble</t>
-  </si>
-  <si>
-    <t>7.9596</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
-    <t>Canadian Dollar</t>
-  </si>
-  <si>
-    <t>12.969</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>756</t>
-  </si>
-  <si>
-    <t>CHF</t>
-  </si>
-  <si>
-    <t>Swiss Franc</t>
-  </si>
-  <si>
-    <t>17.4096</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>156</t>
-  </si>
-  <si>
-    <t>CNY</t>
-  </si>
-  <si>
-    <t>Chinese yuan renminbi</t>
-  </si>
-  <si>
-    <t>2.5385</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>CZK</t>
-  </si>
-  <si>
-    <t>Czech Koruna</t>
-  </si>
-  <si>
-    <t>0.771</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>208</t>
-  </si>
-  <si>
-    <t>DKK</t>
-  </si>
-  <si>
-    <t>Danish Krone</t>
-  </si>
-  <si>
-    <t>2.6443</t>
+    <t>46</t>
+  </si>
+  <si>
+    <t>960</t>
+  </si>
+  <si>
+    <t>XDR</t>
+  </si>
+  <si>
+    <t>Special Drawing Rights</t>
+  </si>
+  <si>
+    <t>23.9515</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>860</t>
+  </si>
+  <si>
+    <t>UZS</t>
+  </si>
+  <si>
+    <t>Uzbekistan Sum</t>
+  </si>
+  <si>
+    <t>0.2032</t>
   </si>
   <si>
     <t>17</t>
@@ -298,376 +667,106 @@
     <t>21.9534</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>981</t>
-  </si>
-  <si>
-    <t>GEL</t>
-  </si>
-  <si>
-    <t>Georgian Lar</t>
-  </si>
-  <si>
-    <t>6.4181</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>344</t>
-  </si>
-  <si>
-    <t>HKD</t>
-  </si>
-  <si>
-    <t>Hong Kong dollar</t>
-  </si>
-  <si>
-    <t>2.183</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>191</t>
-  </si>
-  <si>
-    <t>HRK</t>
-  </si>
-  <si>
-    <t>Croatian Kuna</t>
-  </si>
-  <si>
-    <t>2.6575</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>348</t>
-  </si>
-  <si>
-    <t>HUF</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Hungarian Forint</t>
-  </si>
-  <si>
-    <t>6.1386</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>376</t>
-  </si>
-  <si>
-    <t>ILS</t>
-  </si>
-  <si>
-    <t>Shekel Israelit</t>
-  </si>
-  <si>
-    <t>4.6736</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>356</t>
-  </si>
-  <si>
-    <t>INR</t>
-  </si>
-  <si>
-    <t>Indian rupee</t>
-  </si>
-  <si>
-    <t>2.4281</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>352</t>
-  </si>
-  <si>
-    <t>ISK</t>
-  </si>
-  <si>
-    <t>Iceland Krona</t>
-  </si>
-  <si>
-    <t>1.4292</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>392</t>
-  </si>
-  <si>
-    <t>JPY</t>
-  </si>
-  <si>
-    <t>Japanese Yen</t>
-  </si>
-  <si>
-    <t>15.8045</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>417</t>
-  </si>
-  <si>
-    <t>KGS</t>
-  </si>
-  <si>
-    <t>Kyrgyzstan Som</t>
-  </si>
-  <si>
-    <t>2.4506</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>410</t>
-  </si>
-  <si>
-    <t>KRW</t>
-  </si>
-  <si>
-    <t>South Korean won</t>
-  </si>
-  <si>
-    <t>1.5333</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>414</t>
-  </si>
-  <si>
-    <t>KWD</t>
-  </si>
-  <si>
-    <t>Kuwaiti Dinar</t>
-  </si>
-  <si>
-    <t>56.5331</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>398</t>
-  </si>
-  <si>
-    <t>KZT</t>
-  </si>
-  <si>
-    <t>Kazakhstan Tenge</t>
-  </si>
-  <si>
-    <t>0.4546</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>807</t>
-  </si>
-  <si>
-    <t>MKD</t>
-  </si>
-  <si>
-    <t>Macedonian denar</t>
-  </si>
-  <si>
-    <t>3.2053</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>458</t>
-  </si>
-  <si>
-    <t>MYR</t>
-  </si>
-  <si>
-    <t>Malaysian Ringgit</t>
-  </si>
-  <si>
-    <t>4.18</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>578</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>Norwegian Krone</t>
-  </si>
-  <si>
-    <t>2.0248</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>554</t>
-  </si>
-  <si>
-    <t>NZD</t>
-  </si>
-  <si>
-    <t>New Zealand Dollar</t>
-  </si>
-  <si>
-    <t>11.6987</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>985</t>
-  </si>
-  <si>
-    <t>PLN</t>
-  </si>
-  <si>
-    <t>Polish Zloty</t>
-  </si>
-  <si>
-    <t>4.5941</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>941</t>
-  </si>
-  <si>
-    <t>RSD</t>
-  </si>
-  <si>
-    <t>Serbian Dinar</t>
-  </si>
-  <si>
-    <t>16.6691</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>752</t>
-  </si>
-  <si>
-    <t>SEK</t>
-  </si>
-  <si>
-    <t>Swedish Krona</t>
-  </si>
-  <si>
-    <t>1.9297</t>
-  </si>
-  <si>
-    <t>972</t>
-  </si>
-  <si>
-    <t>TJS</t>
-  </si>
-  <si>
-    <t>Tajikistan Somoni</t>
-  </si>
-  <si>
-    <t>1.8146</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>934</t>
-  </si>
-  <si>
-    <t>TMT</t>
-  </si>
-  <si>
-    <t>Turkmenistan Manat</t>
-  </si>
-  <si>
-    <t>4.8906</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>949</t>
-  </si>
-  <si>
-    <t>TRY</t>
-  </si>
-  <si>
-    <t>Turkish Lira</t>
-  </si>
-  <si>
-    <t>3.1455</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>860</t>
-  </si>
-  <si>
-    <t>UZS</t>
-  </si>
-  <si>
-    <t>Uzbekistan Sum</t>
-  </si>
-  <si>
-    <t>0.2032</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>960</t>
-  </si>
-  <si>
-    <t>XDR</t>
-  </si>
-  <si>
-    <t>Special Drawing Rights</t>
-  </si>
-  <si>
-    <t>23.9515</t>
+    <t>1.567</t>
+  </si>
+  <si>
+    <t>17.1278</t>
+  </si>
+  <si>
+    <t>2.6428</t>
+  </si>
+  <si>
+    <t>0.7683</t>
+  </si>
+  <si>
+    <t>0.4516</t>
+  </si>
+  <si>
+    <t>11.6769</t>
+  </si>
+  <si>
+    <t>4.8937</t>
+  </si>
+  <si>
+    <t>2.4521</t>
+  </si>
+  <si>
+    <t>16.5909</t>
+  </si>
+  <si>
+    <t>10.1055</t>
+  </si>
+  <si>
+    <t>2.5308</t>
+  </si>
+  <si>
+    <t>10.0445</t>
+  </si>
+  <si>
+    <t>0.3524</t>
+  </si>
+  <si>
+    <t>4.1995</t>
+  </si>
+  <si>
+    <t>2.6321</t>
+  </si>
+  <si>
+    <t>4.6866</t>
+  </si>
+  <si>
+    <t>17.4489</t>
   </si>
   <si>
     <t>19.6456</t>
   </si>
   <si>
-    <t>17.1278</t>
+    <t>2.0054</t>
+  </si>
+  <si>
+    <t>23.9289</t>
+  </si>
+  <si>
+    <t>2.1837</t>
+  </si>
+  <si>
+    <t>0.2033</t>
+  </si>
+  <si>
+    <t>1.8157</t>
+  </si>
+  <si>
+    <t>1.5248</t>
+  </si>
+  <si>
+    <t>3.1921</t>
+  </si>
+  <si>
+    <t>6.4233</t>
+  </si>
+  <si>
+    <t>6.1153</t>
+  </si>
+  <si>
+    <t>12.9023</t>
+  </si>
+  <si>
+    <t>1.4185</t>
   </si>
   <si>
     <t>0.2549</t>
   </si>
   <si>
-    <t>4.1995</t>
+    <t>15.8466</t>
+  </si>
+  <si>
+    <t>2.4147</t>
+  </si>
+  <si>
+    <t>4.1765</t>
+  </si>
+  <si>
+    <t>3.1059</t>
   </si>
   <si>
     <t>0.6113</t>
@@ -676,232 +775,142 @@
     <t>4.6632</t>
   </si>
   <si>
-    <t>1.567</t>
-  </si>
-  <si>
-    <t>0.3524</t>
+    <t>56.5293</t>
   </si>
   <si>
     <t>12.3226</t>
   </si>
   <si>
-    <t>10.1055</t>
-  </si>
-  <si>
-    <t>10.0445</t>
-  </si>
-  <si>
     <t>7.947</t>
   </si>
   <si>
-    <t>12.9023</t>
-  </si>
-  <si>
-    <t>17.4489</t>
-  </si>
-  <si>
-    <t>2.5308</t>
-  </si>
-  <si>
-    <t>0.7683</t>
-  </si>
-  <si>
-    <t>2.6321</t>
-  </si>
-  <si>
     <t>22.052</t>
   </si>
   <si>
-    <t>6.4233</t>
-  </si>
-  <si>
-    <t>2.1837</t>
-  </si>
-  <si>
-    <t>2.6428</t>
-  </si>
-  <si>
-    <t>6.1153</t>
-  </si>
-  <si>
-    <t>4.6866</t>
-  </si>
-  <si>
-    <t>2.4147</t>
-  </si>
-  <si>
-    <t>1.4185</t>
-  </si>
-  <si>
-    <t>15.8466</t>
-  </si>
-  <si>
-    <t>2.4521</t>
-  </si>
-  <si>
-    <t>1.5248</t>
-  </si>
-  <si>
-    <t>56.5293</t>
-  </si>
-  <si>
-    <t>0.4516</t>
-  </si>
-  <si>
-    <t>3.1921</t>
-  </si>
-  <si>
-    <t>4.1765</t>
-  </si>
-  <si>
-    <t>2.0054</t>
-  </si>
-  <si>
-    <t>11.6769</t>
+    <t>1.9168</t>
   </si>
   <si>
     <t>4.576</t>
   </si>
   <si>
-    <t>16.5909</t>
-  </si>
-  <si>
-    <t>1.9168</t>
-  </si>
-  <si>
-    <t>1.8157</t>
-  </si>
-  <si>
-    <t>4.8937</t>
-  </si>
-  <si>
-    <t>3.1059</t>
-  </si>
-  <si>
-    <t>0.2033</t>
-  </si>
-  <si>
-    <t>23.9289</t>
+    <t>2.638</t>
+  </si>
+  <si>
+    <t>17.1423</t>
+  </si>
+  <si>
+    <t>17.3804</t>
+  </si>
+  <si>
+    <t>11.6936</t>
+  </si>
+  <si>
+    <t>4.8978</t>
+  </si>
+  <si>
+    <t>7.9454</t>
+  </si>
+  <si>
+    <t>3.1826</t>
+  </si>
+  <si>
+    <t>22.0398</t>
+  </si>
+  <si>
+    <t>1.5295</t>
+  </si>
+  <si>
+    <t>56.5678</t>
+  </si>
+  <si>
+    <t>2.0069</t>
+  </si>
+  <si>
+    <t>6.4402</t>
+  </si>
+  <si>
+    <t>4.5661</t>
+  </si>
+  <si>
+    <t>12.923</t>
+  </si>
+  <si>
+    <t>16.546</t>
+  </si>
+  <si>
+    <t>1.8165</t>
+  </si>
+  <si>
+    <t>1.4149</t>
+  </si>
+  <si>
+    <t>4.1855</t>
+  </si>
+  <si>
+    <t>0.2555</t>
+  </si>
+  <si>
+    <t>0.7667</t>
+  </si>
+  <si>
+    <t>15.8176</t>
+  </si>
+  <si>
+    <t>1.9131</t>
   </si>
   <si>
     <t>19.5946</t>
   </si>
   <si>
-    <t>17.1423</t>
-  </si>
-  <si>
-    <t>0.2555</t>
-  </si>
-  <si>
-    <t>4.1855</t>
-  </si>
-  <si>
     <t>0.6088</t>
   </si>
   <si>
+    <t>3.1494</t>
+  </si>
+  <si>
+    <t>2.6253</t>
+  </si>
+  <si>
+    <t>23.9186</t>
+  </si>
+  <si>
+    <t>10.0183</t>
+  </si>
+  <si>
+    <t>2.5357</t>
+  </si>
+  <si>
+    <t>12.3382</t>
+  </si>
+  <si>
+    <t>10.1132</t>
+  </si>
+  <si>
+    <t>4.6655</t>
+  </si>
+  <si>
+    <t>4.1747</t>
+  </si>
+  <si>
     <t>4.6672</t>
   </si>
   <si>
+    <t>2.4136</t>
+  </si>
+  <si>
+    <t>0.453</t>
+  </si>
+  <si>
     <t>1.5701</t>
   </si>
   <si>
-    <t>12.3382</t>
-  </si>
-  <si>
-    <t>10.1132</t>
-  </si>
-  <si>
-    <t>10.0183</t>
-  </si>
-  <si>
-    <t>7.9454</t>
-  </si>
-  <si>
-    <t>12.923</t>
-  </si>
-  <si>
-    <t>17.3804</t>
-  </si>
-  <si>
-    <t>2.5357</t>
-  </si>
-  <si>
-    <t>0.7667</t>
-  </si>
-  <si>
-    <t>2.6253</t>
-  </si>
-  <si>
-    <t>22.0398</t>
-  </si>
-  <si>
-    <t>6.4402</t>
-  </si>
-  <si>
     <t>2.1858</t>
   </si>
   <si>
-    <t>2.638</t>
+    <t>2.4548</t>
   </si>
   <si>
     <t>6.0758</t>
-  </si>
-  <si>
-    <t>4.6655</t>
-  </si>
-  <si>
-    <t>2.4136</t>
-  </si>
-  <si>
-    <t>1.4149</t>
-  </si>
-  <si>
-    <t>15.8176</t>
-  </si>
-  <si>
-    <t>2.4548</t>
-  </si>
-  <si>
-    <t>1.5295</t>
-  </si>
-  <si>
-    <t>56.5678</t>
-  </si>
-  <si>
-    <t>0.453</t>
-  </si>
-  <si>
-    <t>3.1826</t>
-  </si>
-  <si>
-    <t>4.1747</t>
-  </si>
-  <si>
-    <t>2.0069</t>
-  </si>
-  <si>
-    <t>11.6936</t>
-  </si>
-  <si>
-    <t>4.5661</t>
-  </si>
-  <si>
-    <t>16.546</t>
-  </si>
-  <si>
-    <t>1.9131</t>
-  </si>
-  <si>
-    <t>1.8165</t>
-  </si>
-  <si>
-    <t>4.8978</t>
-  </si>
-  <si>
-    <t>3.1494</t>
-  </si>
-  <si>
-    <t>23.9186</t>
   </si>
 </sst>
 </file>
@@ -1115,27 +1124,27 @@
         <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
@@ -1146,702 +1155,702 @@
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
         <v>56</v>
       </c>
-      <c r="C12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G21" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G23" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G24" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G25" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G26" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G27" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G28" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>35</v>
       </c>
       <c r="F29" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G29" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E30" t="s">
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G30" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E31" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G31" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D32" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F32" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G32" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F33" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G33" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E34" t="s">
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G34" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C35" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G35" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D36" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F36" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C37" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F37" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G37" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D38" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E38" t="s">
         <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G38" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>43</v>
+        <v>192</v>
       </c>
       <c r="C39" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E39" t="s">
         <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="G39" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C40" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D40" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E40" t="s">
         <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G40" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C41" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E41" t="s">
         <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="G41" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C42" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D42" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E42" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="F42" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G42" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C43" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D43" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E43" t="s">
         <v>9</v>
       </c>
       <c r="F43" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="G43" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -1887,842 +1896,842 @@
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="G5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>177</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>178</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>179</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="G9" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>164</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>165</v>
       </c>
       <c r="G10" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>51</v>
+        <v>192</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>194</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>195</v>
       </c>
       <c r="G11" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>61</v>
+        <v>197</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>198</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>199</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>200</v>
       </c>
       <c r="G13" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="G14" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="G15" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>75</v>
+        <v>172</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>174</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>175</v>
       </c>
       <c r="G16" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="G17" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>89</v>
+        <v>167</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>168</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>169</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>170</v>
       </c>
       <c r="G19" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="G20" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>99</v>
+        <v>202</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>203</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>204</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>205</v>
       </c>
       <c r="G21" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
         <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="G22" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>109</v>
+        <v>207</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>208</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>113</v>
+        <v>210</v>
       </c>
       <c r="G23" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="G24" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="G25" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="G26" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>133</v>
+        <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>135</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="G29" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F30" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
       <c r="G30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>189</v>
       </c>
       <c r="E31" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="G31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>155</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
-        <v>157</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F32" t="s">
-        <v>158</v>
+        <v>57</v>
       </c>
       <c r="G32" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>160</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>91</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F33" t="s">
-        <v>163</v>
+        <v>92</v>
       </c>
       <c r="G33" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="E34" t="s">
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="G34" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>170</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>171</v>
+        <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>173</v>
+        <v>67</v>
       </c>
       <c r="G35" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>175</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>176</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
       <c r="E36" t="s">
         <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>178</v>
+        <v>82</v>
       </c>
       <c r="G36" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>181</v>
+        <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
+        <v>115</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F37" t="s">
-        <v>183</v>
+        <v>116</v>
       </c>
       <c r="G37" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>185</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>187</v>
+        <v>130</v>
       </c>
       <c r="E38" t="s">
         <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>188</v>
+        <v>131</v>
       </c>
       <c r="G38" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>43</v>
+        <v>152</v>
       </c>
       <c r="C39" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="E39" t="s">
         <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="G39" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="D40" t="s">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="E40" t="s">
         <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="G40" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="C41" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E41" t="s">
         <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="G41" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="C42" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="D42" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="E42" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F42" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="G42" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>209</v>
+        <v>98</v>
       </c>
       <c r="C43" t="s">
-        <v>210</v>
+        <v>99</v>
       </c>
       <c r="D43" t="s">
-        <v>211</v>
+        <v>100</v>
       </c>
       <c r="E43" t="s">
         <v>9</v>
       </c>
       <c r="F43" t="s">
-        <v>212</v>
+        <v>101</v>
       </c>
       <c r="G43" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2768,842 +2777,842 @@
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
       <c r="G7" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>160</v>
       </c>
       <c r="G8" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>213</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>214</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>215</v>
       </c>
       <c r="G9" t="s">
-        <v>221</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="G10" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="G11" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="G12" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="G14" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>75</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>163</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>165</v>
       </c>
       <c r="G16" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="G17" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="G18" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>94</v>
+        <v>187</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>188</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>189</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>190</v>
       </c>
       <c r="G20" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G21" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="G22" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>109</v>
+        <v>182</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>113</v>
+        <v>185</v>
       </c>
       <c r="G23" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>115</v>
+        <v>167</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>168</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>169</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="G24" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="G25" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>127</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
       <c r="G26" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="E27" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="G27" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>135</v>
+        <v>202</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>203</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>138</v>
+        <v>205</v>
       </c>
       <c r="G28" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>140</v>
+        <v>197</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>198</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>199</v>
       </c>
       <c r="E29" t="s">
-        <v>112</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>143</v>
+        <v>200</v>
       </c>
       <c r="G29" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>145</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>50</v>
       </c>
       <c r="E30" t="s">
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>148</v>
+        <v>51</v>
       </c>
       <c r="G30" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E31" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G31" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="D32" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
       <c r="G32" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
       </c>
       <c r="F33" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="G33" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="E34" t="s">
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="G34" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>170</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>171</v>
+        <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>115</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>173</v>
+        <v>116</v>
       </c>
       <c r="G35" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>176</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>177</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F36" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="G36" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>180</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>181</v>
+        <v>39</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
+        <v>40</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>35</v>
       </c>
       <c r="F37" t="s">
-        <v>183</v>
+        <v>41</v>
       </c>
       <c r="G37" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>185</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>186</v>
+        <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>187</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F38" t="s">
-        <v>188</v>
+        <v>36</v>
       </c>
       <c r="G38" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>190</v>
+        <v>143</v>
       </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="E39" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F39" t="s">
-        <v>192</v>
+        <v>145</v>
       </c>
       <c r="G39" t="s">
-        <v>292</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="C40" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="D40" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F40" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="G40" t="s">
-        <v>293</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>199</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
+        <v>76</v>
       </c>
       <c r="E41" t="s">
         <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>202</v>
+        <v>77</v>
       </c>
       <c r="G41" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="C42" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="D42" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="E42" t="s">
-        <v>112</v>
+        <v>35</v>
       </c>
       <c r="F42" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="G42" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>209</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>210</v>
+        <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>211</v>
+        <v>61</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F43" t="s">
-        <v>212</v>
+        <v>62</v>
       </c>
       <c r="G43" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>